<commit_message>
Review Research Papers, ARIMA forecasts, reorganize notebooks, write evaluate_model function
</commit_message>
<xml_diff>
--- a/data/flu_cases/flu_cases_2022_2023.xlsx
+++ b/data/flu_cases/flu_cases_2022_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projects\LHL_final_project_influenza_forecasting\data\flu_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7164736-3044-4A2E-93D1-FA76C6D502D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD1C286-DE8F-4F7D-A4F0-DCB89CACDAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37575" yWindow="2955" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30435" yWindow="930" windowWidth="17310" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,7 +521,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1">
         <v>20</v>
@@ -587,10 +587,10 @@
         <v>41</v>
       </c>
       <c r="B8" s="1">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C8" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="1">
         <v>20</v>
@@ -610,10 +610,10 @@
         <v>42</v>
       </c>
       <c r="B9" s="1">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="C9" s="1">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D9" s="1">
         <v>11</v>
@@ -622,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="1">
-        <v>2.7</v>
+        <v>2.4</v>
       </c>
       <c r="G9" s="1">
         <v>0.1</v>
@@ -633,19 +633,19 @@
         <v>43</v>
       </c>
       <c r="B10" s="1">
-        <v>495</v>
+        <v>407</v>
       </c>
       <c r="C10" s="1">
-        <v>524</v>
+        <v>595</v>
       </c>
       <c r="D10" s="1">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1">
         <v>6</v>
       </c>
       <c r="F10" s="1">
-        <v>6.4</v>
+        <v>5.6</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -656,19 +656,19 @@
         <v>44</v>
       </c>
       <c r="B11" s="1">
-        <v>1083</v>
+        <v>995</v>
       </c>
       <c r="C11" s="1">
-        <v>1149</v>
+        <v>1351</v>
       </c>
       <c r="D11" s="1">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F11" s="1">
-        <v>11.6</v>
+        <v>10.9</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -679,21 +679,44 @@
         <v>45</v>
       </c>
       <c r="B12" s="1">
-        <v>1846</v>
+        <v>1799</v>
       </c>
       <c r="C12" s="1">
-        <v>1807</v>
+        <v>2265</v>
       </c>
       <c r="D12" s="1">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E12" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="1">
-        <v>15.6</v>
+        <v>16</v>
       </c>
       <c r="G12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>46</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3159</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2213</v>
+      </c>
+      <c r="D13" s="1">
+        <v>73</v>
+      </c>
+      <c r="E13" s="1">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="G13" s="1">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
re-factor code, organize notebooks, work on visualizations
</commit_message>
<xml_diff>
--- a/data/flu_cases/flu_cases_2022_2023.xlsx
+++ b/data/flu_cases/flu_cases_2022_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projects\LHL_final_project_influenza_forecasting\data\flu_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD1C286-DE8F-4F7D-A4F0-DCB89CACDAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6339707F-9FFF-4B62-9DDF-CB059BF500E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30435" yWindow="930" windowWidth="17310" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36375" yWindow="4260" windowWidth="17310" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,6 +718,29 @@
       </c>
       <c r="G13" s="1">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5424</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2214</v>
+      </c>
+      <c r="D14" s="1">
+        <v>119</v>
+      </c>
+      <c r="E14" s="1">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1">
+        <v>23.1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>